<commit_message>
[UPDATE]add userinfo address, multiple time purchase
</commit_message>
<xml_diff>
--- a/project/preprocessing/DataGenerator/category_code.xlsx
+++ b/project/preprocessing/DataGenerator/category_code.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pgm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egn\Desktop\GitHub\KUSW\project\preprocessing\DataGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5446977-F32C-4769-BA13-52D08C031D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3406824-3323-4C50-A332-59F115118A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>coupang</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,10 +180,6 @@
   </si>
   <si>
     <t>고양이 하우스/방석</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>고양이 급식기/급수기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -525,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -949,10 +945,10 @@
         <v>39</v>
       </c>
       <c r="B38">
-        <v>119561</v>
+        <v>157054</v>
       </c>
       <c r="C38">
-        <v>50006734</v>
+        <v>50006728</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -960,10 +956,10 @@
         <v>40</v>
       </c>
       <c r="B39">
-        <v>157054</v>
+        <v>119558</v>
       </c>
       <c r="C39">
-        <v>50006728</v>
+        <v>50006694</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -971,10 +967,10 @@
         <v>41</v>
       </c>
       <c r="B40">
-        <v>119558</v>
+        <v>385076</v>
       </c>
       <c r="C40">
-        <v>50006694</v>
+        <v>50006662</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -982,20 +978,9 @@
         <v>42</v>
       </c>
       <c r="B41">
-        <v>385076</v>
+        <v>119568</v>
       </c>
       <c r="C41">
-        <v>50006662</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42">
-        <v>119568</v>
-      </c>
-      <c r="C42">
         <v>50006718</v>
       </c>
     </row>

</xml_diff>